<commit_message>
added data classes, changed requirements
</commit_message>
<xml_diff>
--- a/doc/Anforderungsliste.xlsx
+++ b/doc/Anforderungsliste.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
-    <sheet name="Ziele" sheetId="1" r:id="rId1"/>
-    <sheet name="Anforderungen" sheetId="2" r:id="rId2"/>
+    <sheet name="Vision" sheetId="5" r:id="rId1"/>
+    <sheet name="Ziele" sheetId="1" r:id="rId2"/>
+    <sheet name="Anforderungen" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -556,7 +557,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="102">
   <si>
     <t>Nummer</t>
   </si>
@@ -687,9 +688,6 @@
     <t>Bezeichnung</t>
   </si>
   <si>
-    <t>…</t>
-  </si>
-  <si>
     <t>4.1</t>
   </si>
   <si>
@@ -817,6 +815,54 @@
   </si>
   <si>
     <t>4.4.1</t>
+  </si>
+  <si>
+    <t>Mögliche Schwachstellen in einem Verkehrsnetz erkennen.</t>
+  </si>
+  <si>
+    <t>Statistische Daten anhand einer Simulation über ein bestimmtes Verkehrsszenario erheben.</t>
+  </si>
+  <si>
+    <t>Simulation realer Verkehrsnetze.</t>
+  </si>
+  <si>
+    <t>1, 2, 3</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1, 2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Vision</t>
+  </si>
+  <si>
+    <t>Agent-basierte Mikrosimulation auf realen Verkehrsnetzen für den einfachen User ermöglichen.</t>
+  </si>
+  <si>
+    <t>Verschiedene Fahrertypen können simuliert werden.</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>1, 3</t>
+  </si>
+  <si>
+    <t>Scope</t>
+  </si>
+  <si>
+    <t>Überholen nicht auf Gegenfahrban möglich</t>
+  </si>
+  <si>
+    <t>Kein Editor. Daten-Import</t>
   </si>
 </sst>
 </file>
@@ -1231,37 +1277,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="75.5703125" customWidth="1"/>
+    <col min="1" max="1" width="93.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>43</v>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A8" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1270,10 +1329,74 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="93.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1286,12 +1409,12 @@
     <col min="7" max="10" width="3.85546875" style="2" customWidth="1"/>
     <col min="11" max="11" width="19.85546875" customWidth="1"/>
     <col min="12" max="12" width="10.5703125" style="5" customWidth="1"/>
-    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="13" max="13" width="13" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -1301,8 +1424,9 @@
       <c r="I1" s="16"/>
       <c r="J1" s="16"/>
       <c r="L1" s="17"/>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M1" s="15"/>
+    </row>
+    <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -1335,11 +1459,19 @@
       <c r="L3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -1356,9 +1488,15 @@
       <c r="J5" s="4"/>
       <c r="K5" s="3"/>
       <c r="L5" s="6"/>
-      <c r="M5" s="3"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M5" s="8"/>
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>1.1000000000000001</v>
       </c>
@@ -1390,8 +1528,17 @@
       <c r="L6" s="5">
         <v>41907</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M6" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>1.2</v>
       </c>
@@ -1414,7 +1561,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" ref="J7:J13" si="0">AVERAGE(G7:I7)</f>
+        <f t="shared" ref="J7:J12" si="0">AVERAGE(G7:I7)</f>
         <v>1.6666666666666667</v>
       </c>
       <c r="K7" t="s">
@@ -1423,8 +1570,11 @@
       <c r="L7" s="5">
         <v>41907</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M7" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>1.3</v>
       </c>
@@ -1456,8 +1606,11 @@
       <c r="L8" s="5">
         <v>41907</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M8" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>1.4</v>
       </c>
@@ -1489,8 +1642,11 @@
       <c r="L9" s="5">
         <v>41907</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M9" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C10" s="7" t="s">
         <v>19</v>
       </c>
@@ -1522,8 +1678,11 @@
       <c r="L10" s="5">
         <v>41907</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M10" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C11" s="7" t="s">
         <v>19</v>
       </c>
@@ -1555,8 +1714,11 @@
       <c r="L11" s="5">
         <v>41907</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M11" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>30</v>
       </c>
@@ -1588,16 +1750,19 @@
       <c r="L12" s="5">
         <v>41907</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M12" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
         <v>51</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="F13" t="s">
         <v>38</v>
@@ -1621,8 +1786,11 @@
       <c r="L13" s="5">
         <v>41907</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M13" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>2</v>
       </c>
@@ -1639,7 +1807,7 @@
       <c r="J16" s="4"/>
       <c r="K16" s="3"/>
       <c r="L16" s="6"/>
-      <c r="M16" s="3"/>
+      <c r="M16" s="8"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
@@ -1673,6 +1841,9 @@
       <c r="L17" s="5">
         <v>41907</v>
       </c>
+      <c r="M17" s="7" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
@@ -1706,13 +1877,16 @@
       <c r="L18" s="5">
         <v>41907</v>
       </c>
+      <c r="M18" s="7" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>22</v>
@@ -1739,6 +1913,9 @@
       <c r="L19" s="5">
         <v>41907</v>
       </c>
+      <c r="M19" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
@@ -1772,6 +1949,9 @@
       <c r="L20" s="5">
         <v>41907</v>
       </c>
+      <c r="M20" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
@@ -1805,13 +1985,16 @@
       <c r="L21" s="5">
         <v>41907</v>
       </c>
+      <c r="M21" s="7" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>22</v>
@@ -1838,10 +2021,13 @@
       <c r="L22" s="5">
         <v>41907</v>
       </c>
+      <c r="M22" s="7" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D23" t="s">
         <v>34</v>
@@ -1870,6 +2056,9 @@
       </c>
       <c r="L23" s="5">
         <v>41907</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -1889,14 +2078,14 @@
       <c r="J26" s="4"/>
       <c r="K26" s="3"/>
       <c r="L26" s="6"/>
-      <c r="M26" s="3"/>
+      <c r="M26" s="8"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>22</v>
@@ -1923,13 +2112,16 @@
       <c r="L27" s="5">
         <v>41907</v>
       </c>
+      <c r="M27" s="7" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>22</v>
@@ -1955,6 +2147,9 @@
       </c>
       <c r="L28" s="5">
         <v>41907</v>
+      </c>
+      <c r="M28" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -1962,7 +2157,7 @@
         <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>22</v>
@@ -1989,13 +2184,16 @@
       <c r="L29" s="5">
         <v>41907</v>
       </c>
+      <c r="M29" s="7" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C30" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" t="s">
         <v>60</v>
-      </c>
-      <c r="D30" t="s">
-        <v>61</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>22</v>
@@ -2022,13 +2220,16 @@
       <c r="L30" s="5">
         <v>41907</v>
       </c>
+      <c r="M30" s="7" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C31" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" t="s">
         <v>62</v>
-      </c>
-      <c r="D31" t="s">
-        <v>63</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>22</v>
@@ -2055,13 +2256,16 @@
       <c r="L31" s="5">
         <v>41907</v>
       </c>
+      <c r="M31" s="7" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>22</v>
@@ -2088,13 +2292,16 @@
       <c r="L32" s="5">
         <v>41907</v>
       </c>
+      <c r="M32" s="7" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" t="s">
         <v>69</v>
-      </c>
-      <c r="D33" t="s">
-        <v>70</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>22</v>
@@ -2120,6 +2327,9 @@
       </c>
       <c r="L33" s="5">
         <v>41907</v>
+      </c>
+      <c r="M33" s="7" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -2139,14 +2349,14 @@
       <c r="J36" s="4"/>
       <c r="K36" s="3"/>
       <c r="L36" s="6"/>
-      <c r="M36" s="3"/>
+      <c r="M36" s="8"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B37" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D37" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>22</v>
@@ -2173,13 +2383,16 @@
       <c r="L37" s="5">
         <v>41907</v>
       </c>
+      <c r="M37" s="7" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>37</v>
@@ -2206,13 +2419,16 @@
       <c r="L38" s="5">
         <v>41907</v>
       </c>
+      <c r="M38" s="7" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B39" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>37</v>
@@ -2239,13 +2455,16 @@
       <c r="L39" s="5">
         <v>41907</v>
       </c>
+      <c r="M39" s="7" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B40" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>22</v>
@@ -2272,13 +2491,16 @@
       <c r="L40" s="5">
         <v>41907</v>
       </c>
+      <c r="M40" s="7" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C41" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>22</v>
@@ -2304,6 +2526,9 @@
       </c>
       <c r="L41" s="5">
         <v>41907</v>
+      </c>
+      <c r="M41" s="7" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -2323,14 +2548,14 @@
       <c r="J44" s="4"/>
       <c r="K44" s="3"/>
       <c r="L44" s="6"/>
-      <c r="M44" s="3"/>
+      <c r="M44" s="8"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B45" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>37</v>
@@ -2357,13 +2582,16 @@
       <c r="L45" s="5">
         <v>41907</v>
       </c>
+      <c r="M45" s="7" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B46" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D46" t="s">
         <v>72</v>
-      </c>
-      <c r="D46" t="s">
-        <v>73</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>22</v>
@@ -2390,13 +2618,16 @@
       <c r="L46" s="5">
         <v>41907</v>
       </c>
+      <c r="M46" s="7" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C47" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D47" t="s">
         <v>74</v>
-      </c>
-      <c r="D47" t="s">
-        <v>75</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>22</v>
@@ -2423,13 +2654,16 @@
       <c r="L47" s="5">
         <v>41907</v>
       </c>
+      <c r="M47" s="7" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C48" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>22</v>
@@ -2456,13 +2690,16 @@
       <c r="L48" s="5">
         <v>41907</v>
       </c>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M48" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B49" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D49" t="s">
         <v>76</v>
-      </c>
-      <c r="D49" t="s">
-        <v>77</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>22</v>
@@ -2489,13 +2726,16 @@
       <c r="L49" s="5">
         <v>41907</v>
       </c>
-    </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M49" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C50" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D50" t="s">
         <v>78</v>
-      </c>
-      <c r="D50" t="s">
-        <v>79</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>22</v>
@@ -2522,13 +2762,16 @@
       <c r="L50" s="5">
         <v>41907</v>
       </c>
-    </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M50" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C51" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>22</v>
@@ -2554,6 +2797,9 @@
       </c>
       <c r="L51" s="5">
         <v>41907</v>
+      </c>
+      <c r="M51" s="7" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>